<commit_message>
feat: export qiv to xlsx
</commit_message>
<xml_diff>
--- a/rrggweb/resources/report_quotations.xlsx
+++ b/rrggweb/resources/report_quotations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wrabi\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Riesgos\riesgosgenerales\rrggweb\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04671E7F-7C29-48AE-B941-2277CDF5DF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="1950" yWindow="135" windowWidth="19395" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -247,22 +248,22 @@
     <t xml:space="preserve">USO </t>
   </si>
   <si>
-    <t>PARTICULAR</t>
-  </si>
-  <si>
-    <t>PINTO CRUZ DELFOR</t>
-  </si>
-  <si>
     <t>KIA</t>
   </si>
   <si>
     <t>NIRO</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS</t>
+  </si>
+  <si>
+    <t>TIPO DE USO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$$-1409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
@@ -660,12 +661,114 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,108 +777,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1426,11 +1427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="Q48" sqref="Q48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1474,7 +1475,7 @@
         <v>58</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1483,7 +1484,7 @@
       </c>
       <c r="I6" s="66">
         <f ca="1">TODAY()</f>
-        <v>45119</v>
+        <v>45130</v>
       </c>
       <c r="L6" s="69"/>
       <c r="M6" s="67"/>
@@ -1494,7 +1495,7 @@
         <v>59</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1506,7 +1507,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1529,7 +1530,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1539,7 +1540,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="26">
-        <v>38200</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1559,16 +1560,16 @@
     <row r="12" spans="2:18" ht="75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="29"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="91"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="91"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="92"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="71"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="6" t="s">
@@ -1577,23 +1578,23 @@
       <c r="C13" s="11"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7">
-        <v>994.19</v>
+        <v>0</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7">
-        <v>976.23</v>
+        <v>0</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="7">
-        <v>1146</v>
+        <v>0</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="7">
-        <v>1153.1400000000001</v>
+        <v>0</v>
       </c>
       <c r="L13" s="32"/>
       <c r="M13" s="7">
-        <v>1201</v>
+        <v>0</v>
       </c>
       <c r="R13"/>
     </row>
@@ -1605,27 +1606,27 @@
       <c r="D14" s="6"/>
       <c r="E14" s="7">
         <f>0.03*E13</f>
-        <v>29.825700000000001</v>
+        <v>0</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="7">
         <f>0.03*G13</f>
-        <v>29.286899999999999</v>
+        <v>0</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="7">
         <f>0.03*I13</f>
-        <v>34.379999999999995</v>
+        <v>0</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="7">
         <f>0.03*K13</f>
-        <v>34.594200000000001</v>
+        <v>0</v>
       </c>
       <c r="L14" s="32"/>
       <c r="M14" s="7">
         <f>0.03*M13</f>
-        <v>36.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:18">
@@ -1636,27 +1637,27 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7">
         <f>0.18*(E13+E14)</f>
-        <v>184.32282600000002</v>
+        <v>0</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="7">
         <f>0.18*(G13+G14)</f>
-        <v>180.99304199999997</v>
+        <v>0</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="7">
         <f>0.18*(I13+I14)</f>
-        <v>212.4684</v>
+        <v>0</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="7">
         <f>0.18*(K13+K14)</f>
-        <v>213.79215600000001</v>
+        <v>0</v>
       </c>
       <c r="L15" s="32"/>
       <c r="M15" s="7">
         <f>0.18*(M13+M14)</f>
-        <v>222.66539999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:18">
@@ -1667,44 +1668,44 @@
       <c r="D16" s="47"/>
       <c r="E16" s="49">
         <f>SUM(E13:E15)</f>
-        <v>1208.3385260000002</v>
+        <v>0</v>
       </c>
       <c r="F16" s="50"/>
       <c r="G16" s="49">
         <f>SUM(G13:G15)</f>
-        <v>1186.5099419999999</v>
+        <v>0</v>
       </c>
       <c r="H16" s="50"/>
       <c r="I16" s="49">
         <f>SUM(I13:I15)</f>
-        <v>1392.8484000000001</v>
+        <v>0</v>
       </c>
       <c r="J16" s="50"/>
       <c r="K16" s="49">
         <f>SUM(K13:K15)</f>
-        <v>1401.5263560000001</v>
+        <v>0</v>
       </c>
       <c r="L16" s="50"/>
       <c r="M16" s="49">
         <f>SUM(M13:M15)</f>
-        <v>1459.6954000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="33" customHeight="1">
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="96"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="75"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="27"/>
@@ -1725,26 +1726,26 @@
         <v>5</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="84"/>
-      <c r="F19" s="83" t="s">
+      <c r="E19" s="80"/>
+      <c r="F19" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="84"/>
-      <c r="H19" s="83" t="s">
+      <c r="G19" s="80"/>
+      <c r="H19" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="84"/>
-      <c r="J19" s="83" t="s">
+      <c r="I19" s="80"/>
+      <c r="J19" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="84"/>
-      <c r="L19" s="83" t="s">
+      <c r="K19" s="80"/>
+      <c r="L19" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="M19" s="84"/>
+      <c r="M19" s="80"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="14" t="s">
@@ -1797,26 +1798,26 @@
         <v>9</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="70">
+      <c r="D23" s="100">
         <v>100000</v>
       </c>
-      <c r="E23" s="71"/>
-      <c r="F23" s="70">
+      <c r="E23" s="101"/>
+      <c r="F23" s="100">
         <v>180000</v>
       </c>
-      <c r="G23" s="71"/>
-      <c r="H23" s="70">
+      <c r="G23" s="101"/>
+      <c r="H23" s="100">
         <v>150000</v>
       </c>
-      <c r="I23" s="71"/>
-      <c r="J23" s="70">
+      <c r="I23" s="101"/>
+      <c r="J23" s="100">
         <v>150000</v>
       </c>
-      <c r="K23" s="71"/>
-      <c r="L23" s="70">
+      <c r="K23" s="101"/>
+      <c r="L23" s="100">
         <v>100000</v>
       </c>
-      <c r="M23" s="71"/>
+      <c r="M23" s="101"/>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="9" t="s">
@@ -1827,18 +1828,18 @@
       <c r="E24" s="12"/>
       <c r="F24" s="9"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="81" t="s">
+      <c r="H24" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="82"/>
-      <c r="J24" s="81" t="s">
+      <c r="I24" s="91"/>
+      <c r="J24" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="82"/>
-      <c r="L24" s="81" t="s">
+      <c r="K24" s="91"/>
+      <c r="L24" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="82"/>
+      <c r="M24" s="91"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="14"/>
@@ -1859,52 +1860,52 @@
         <v>9</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="70">
+      <c r="D26" s="100">
         <v>20000</v>
       </c>
-      <c r="E26" s="71"/>
-      <c r="F26" s="70">
+      <c r="E26" s="101"/>
+      <c r="F26" s="100">
         <v>30000</v>
       </c>
-      <c r="G26" s="71"/>
-      <c r="H26" s="70">
+      <c r="G26" s="101"/>
+      <c r="H26" s="100">
         <v>80000</v>
       </c>
-      <c r="I26" s="71"/>
-      <c r="J26" s="70">
+      <c r="I26" s="101"/>
+      <c r="J26" s="100">
         <v>50000</v>
       </c>
-      <c r="K26" s="71"/>
-      <c r="L26" s="70">
+      <c r="K26" s="101"/>
+      <c r="L26" s="100">
         <v>10000</v>
       </c>
-      <c r="M26" s="71"/>
+      <c r="M26" s="101"/>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="82"/>
-      <c r="F27" s="81" t="s">
+      <c r="E27" s="91"/>
+      <c r="F27" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="82"/>
-      <c r="H27" s="81" t="s">
+      <c r="G27" s="91"/>
+      <c r="H27" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="82"/>
-      <c r="J27" s="81" t="s">
+      <c r="I27" s="91"/>
+      <c r="J27" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="82"/>
-      <c r="L27" s="81" t="s">
+      <c r="K27" s="91"/>
+      <c r="L27" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M27" s="82"/>
+      <c r="M27" s="91"/>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="14"/>
@@ -1941,78 +1942,78 @@
         <v>16</v>
       </c>
       <c r="C30" s="15"/>
-      <c r="D30" s="70">
+      <c r="D30" s="100">
         <v>20000</v>
       </c>
-      <c r="E30" s="71"/>
-      <c r="F30" s="70">
+      <c r="E30" s="101"/>
+      <c r="F30" s="100">
         <v>20000</v>
       </c>
-      <c r="G30" s="71"/>
-      <c r="H30" s="70">
+      <c r="G30" s="101"/>
+      <c r="H30" s="100">
         <v>25000</v>
       </c>
-      <c r="I30" s="71"/>
-      <c r="J30" s="70">
+      <c r="I30" s="101"/>
+      <c r="J30" s="100">
         <v>25000</v>
       </c>
-      <c r="K30" s="71"/>
-      <c r="L30" s="70">
+      <c r="K30" s="101"/>
+      <c r="L30" s="100">
         <v>5000</v>
       </c>
-      <c r="M30" s="71"/>
+      <c r="M30" s="101"/>
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="15"/>
-      <c r="D31" s="70">
+      <c r="D31" s="100">
         <v>4000</v>
       </c>
-      <c r="E31" s="71"/>
-      <c r="F31" s="70">
+      <c r="E31" s="101"/>
+      <c r="F31" s="100">
         <v>4000</v>
       </c>
-      <c r="G31" s="71"/>
-      <c r="H31" s="70">
+      <c r="G31" s="101"/>
+      <c r="H31" s="100">
         <v>4000</v>
       </c>
-      <c r="I31" s="71"/>
-      <c r="J31" s="70">
+      <c r="I31" s="101"/>
+      <c r="J31" s="100">
         <v>4000</v>
       </c>
-      <c r="K31" s="71"/>
-      <c r="L31" s="70">
+      <c r="K31" s="101"/>
+      <c r="L31" s="100">
         <v>1000</v>
       </c>
-      <c r="M31" s="71"/>
+      <c r="M31" s="101"/>
     </row>
     <row r="32" spans="2:13">
       <c r="B32" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="15"/>
-      <c r="D32" s="70">
+      <c r="D32" s="100">
         <v>1000</v>
       </c>
-      <c r="E32" s="71"/>
-      <c r="F32" s="70">
+      <c r="E32" s="101"/>
+      <c r="F32" s="100">
         <v>1000</v>
       </c>
-      <c r="G32" s="71"/>
-      <c r="H32" s="70" t="s">
+      <c r="G32" s="101"/>
+      <c r="H32" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="I32" s="71"/>
-      <c r="J32" s="70">
+      <c r="I32" s="101"/>
+      <c r="J32" s="100">
         <v>2000</v>
       </c>
-      <c r="K32" s="71"/>
-      <c r="L32" s="70">
+      <c r="K32" s="101"/>
+      <c r="L32" s="100">
         <v>1000</v>
       </c>
-      <c r="M32" s="71"/>
+      <c r="M32" s="101"/>
     </row>
     <row r="33" spans="2:13" ht="8.25" customHeight="1">
       <c r="B33" s="51"/>
@@ -2033,26 +2034,26 @@
         <v>19</v>
       </c>
       <c r="C34" s="58"/>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="85"/>
-      <c r="F34" s="100" t="s">
+      <c r="E34" s="82"/>
+      <c r="F34" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="86"/>
-      <c r="H34" s="100" t="s">
+      <c r="G34" s="83"/>
+      <c r="H34" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="I34" s="86"/>
-      <c r="J34" s="100" t="s">
+      <c r="I34" s="83"/>
+      <c r="J34" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="86"/>
-      <c r="L34" s="85" t="s">
+      <c r="K34" s="83"/>
+      <c r="L34" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="M34" s="86"/>
+      <c r="M34" s="83"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="9"/>
@@ -2073,110 +2074,110 @@
         <v>21</v>
       </c>
       <c r="C36" s="55"/>
-      <c r="D36" s="75" t="s">
+      <c r="D36" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="76"/>
-      <c r="F36" s="79" t="s">
+      <c r="E36" s="97"/>
+      <c r="F36" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="79"/>
-      <c r="H36" s="75" t="s">
+      <c r="G36" s="104"/>
+      <c r="H36" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="I36" s="76"/>
-      <c r="J36" s="75" t="s">
+      <c r="I36" s="97"/>
+      <c r="J36" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="K36" s="76"/>
-      <c r="L36" s="79" t="s">
+      <c r="K36" s="97"/>
+      <c r="L36" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="M36" s="76"/>
+      <c r="M36" s="97"/>
     </row>
     <row r="37" spans="2:13">
       <c r="B37" s="56" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="57"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="78"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="78"/>
-      <c r="L37" s="80"/>
-      <c r="M37" s="78"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="99"/>
+      <c r="F37" s="105"/>
+      <c r="G37" s="105"/>
+      <c r="H37" s="98"/>
+      <c r="I37" s="99"/>
+      <c r="J37" s="98"/>
+      <c r="K37" s="99"/>
+      <c r="L37" s="105"/>
+      <c r="M37" s="99"/>
     </row>
     <row r="38" spans="2:13">
       <c r="B38" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C38" s="59"/>
-      <c r="D38" s="75" t="s">
+      <c r="D38" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="76"/>
-      <c r="F38" s="75" t="s">
+      <c r="E38" s="97"/>
+      <c r="F38" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="76"/>
-      <c r="H38" s="75" t="s">
+      <c r="G38" s="97"/>
+      <c r="H38" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="76"/>
-      <c r="J38" s="75" t="s">
+      <c r="I38" s="97"/>
+      <c r="J38" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="K38" s="76"/>
-      <c r="L38" s="79" t="s">
+      <c r="K38" s="97"/>
+      <c r="L38" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="M38" s="79"/>
+      <c r="M38" s="104"/>
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="56" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="60"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="78"/>
-      <c r="J39" s="77"/>
-      <c r="K39" s="78"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="80"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="99"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="99"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="99"/>
+      <c r="L39" s="105"/>
+      <c r="M39" s="105"/>
     </row>
     <row r="40" spans="2:13">
       <c r="B40" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="87">
+      <c r="D40" s="93">
         <v>50000</v>
       </c>
-      <c r="E40" s="88"/>
-      <c r="F40" s="87">
+      <c r="E40" s="94"/>
+      <c r="F40" s="93">
         <v>50000</v>
       </c>
-      <c r="G40" s="88"/>
-      <c r="H40" s="89">
+      <c r="G40" s="94"/>
+      <c r="H40" s="102">
         <v>50000</v>
       </c>
-      <c r="I40" s="90"/>
-      <c r="J40" s="87">
+      <c r="I40" s="103"/>
+      <c r="J40" s="93">
         <v>50000</v>
       </c>
-      <c r="K40" s="88"/>
-      <c r="L40" s="108" t="s">
+      <c r="K40" s="94"/>
+      <c r="L40" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="M40" s="88"/>
+      <c r="M40" s="94"/>
     </row>
     <row r="41" spans="2:13">
       <c r="B41" s="9"/>
@@ -2197,56 +2198,56 @@
         <v>27</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="70">
+      <c r="D42" s="100">
         <v>250</v>
       </c>
-      <c r="E42" s="71"/>
-      <c r="F42" s="70">
+      <c r="E42" s="101"/>
+      <c r="F42" s="100">
         <v>250</v>
       </c>
-      <c r="G42" s="71"/>
-      <c r="H42" s="70">
+      <c r="G42" s="101"/>
+      <c r="H42" s="100">
         <v>500</v>
       </c>
-      <c r="I42" s="71"/>
-      <c r="J42" s="70">
+      <c r="I42" s="101"/>
+      <c r="J42" s="100">
         <v>250</v>
       </c>
-      <c r="K42" s="71">
+      <c r="K42" s="101">
         <v>250</v>
       </c>
-      <c r="L42" s="70">
+      <c r="L42" s="100">
         <v>250</v>
       </c>
-      <c r="M42" s="71"/>
+      <c r="M42" s="101"/>
     </row>
     <row r="43" spans="2:13">
       <c r="B43" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="70">
+      <c r="D43" s="100">
         <v>250</v>
       </c>
-      <c r="E43" s="71"/>
-      <c r="F43" s="70">
+      <c r="E43" s="101"/>
+      <c r="F43" s="100">
         <v>250</v>
       </c>
-      <c r="G43" s="71"/>
-      <c r="H43" s="70">
+      <c r="G43" s="101"/>
+      <c r="H43" s="100">
         <v>250</v>
       </c>
-      <c r="I43" s="71"/>
-      <c r="J43" s="70">
+      <c r="I43" s="101"/>
+      <c r="J43" s="100">
         <v>250</v>
       </c>
-      <c r="K43" s="71">
+      <c r="K43" s="101">
         <v>250</v>
       </c>
-      <c r="L43" s="70">
+      <c r="L43" s="100">
         <v>250</v>
       </c>
-      <c r="M43" s="71"/>
+      <c r="M43" s="101"/>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="9"/>
@@ -2267,26 +2268,26 @@
         <v>29</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="70">
+      <c r="D45" s="100">
         <v>1000</v>
       </c>
-      <c r="E45" s="71"/>
-      <c r="F45" s="70">
+      <c r="E45" s="101"/>
+      <c r="F45" s="100">
         <v>500</v>
       </c>
-      <c r="G45" s="71"/>
-      <c r="H45" s="70">
+      <c r="G45" s="101"/>
+      <c r="H45" s="100">
         <v>1000</v>
       </c>
-      <c r="I45" s="71"/>
-      <c r="J45" s="70">
+      <c r="I45" s="101"/>
+      <c r="J45" s="100">
         <v>1000</v>
       </c>
-      <c r="K45" s="71"/>
-      <c r="L45" s="70">
+      <c r="K45" s="101"/>
+      <c r="L45" s="100">
         <v>500</v>
       </c>
-      <c r="M45" s="71"/>
+      <c r="M45" s="101"/>
     </row>
     <row r="46" spans="2:13">
       <c r="B46" s="14"/>
@@ -2307,68 +2308,68 @@
         <v>30</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="81" t="s">
+      <c r="D47" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="82"/>
-      <c r="F47" s="81" t="s">
+      <c r="E47" s="91"/>
+      <c r="F47" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="82"/>
-      <c r="H47" s="81" t="s">
+      <c r="G47" s="91"/>
+      <c r="H47" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="I47" s="82"/>
-      <c r="J47" s="81" t="s">
+      <c r="I47" s="91"/>
+      <c r="J47" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="K47" s="82"/>
-      <c r="L47" s="81" t="s">
+      <c r="K47" s="91"/>
+      <c r="L47" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="M47" s="82"/>
+      <c r="M47" s="91"/>
     </row>
     <row r="48" spans="2:13" ht="44.25" customHeight="1">
       <c r="B48" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C48" s="33"/>
-      <c r="D48" s="81" t="s">
+      <c r="D48" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="82"/>
-      <c r="F48" s="81" t="s">
+      <c r="E48" s="91"/>
+      <c r="F48" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="82"/>
-      <c r="H48" s="81" t="s">
+      <c r="G48" s="91"/>
+      <c r="H48" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="I48" s="82"/>
-      <c r="J48" s="83" t="s">
+      <c r="I48" s="91"/>
+      <c r="J48" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="K48" s="84"/>
-      <c r="L48" s="81" t="s">
+      <c r="K48" s="80"/>
+      <c r="L48" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="M48" s="82"/>
+      <c r="M48" s="91"/>
     </row>
     <row r="49" spans="2:13" ht="19.5" customHeight="1">
-      <c r="B49" s="101" t="s">
+      <c r="B49" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="102"/>
-      <c r="D49" s="102"/>
-      <c r="E49" s="102"/>
-      <c r="F49" s="102"/>
-      <c r="G49" s="102"/>
-      <c r="H49" s="103"/>
-      <c r="I49" s="103"/>
-      <c r="J49" s="102"/>
-      <c r="K49" s="102"/>
-      <c r="L49" s="102"/>
-      <c r="M49" s="104"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="85"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="85"/>
+      <c r="H49" s="86"/>
+      <c r="I49" s="86"/>
+      <c r="J49" s="85"/>
+      <c r="K49" s="85"/>
+      <c r="L49" s="85"/>
+      <c r="M49" s="87"/>
     </row>
     <row r="50" spans="2:13">
       <c r="B50" s="27" t="s">
@@ -2587,36 +2588,36 @@
         <v>46</v>
       </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="81" t="s">
+      <c r="D56" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="E56" s="82"/>
-      <c r="F56" s="81" t="s">
+      <c r="E56" s="91"/>
+      <c r="F56" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="G56" s="82"/>
-      <c r="H56" s="81" t="s">
+      <c r="G56" s="91"/>
+      <c r="H56" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="I56" s="82"/>
-      <c r="J56" s="107" t="s">
+      <c r="I56" s="91"/>
+      <c r="J56" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="K56" s="82"/>
-      <c r="L56" s="81" t="s">
+      <c r="K56" s="91"/>
+      <c r="L56" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="M56" s="82"/>
+      <c r="M56" s="91"/>
     </row>
     <row r="57" spans="2:13" ht="33" customHeight="1">
       <c r="B57" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C57" s="37"/>
-      <c r="D57" s="105" t="s">
+      <c r="D57" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="106"/>
+      <c r="E57" s="89"/>
       <c r="F57" s="20">
         <v>0.2</v>
       </c>
@@ -2643,20 +2644,20 @@
       </c>
     </row>
     <row r="58" spans="2:13" ht="25.5" customHeight="1">
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="73"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="73"/>
-      <c r="M58" s="74"/>
+      <c r="C58" s="107"/>
+      <c r="D58" s="107"/>
+      <c r="E58" s="107"/>
+      <c r="F58" s="107"/>
+      <c r="G58" s="107"/>
+      <c r="H58" s="107"/>
+      <c r="I58" s="107"/>
+      <c r="J58" s="107"/>
+      <c r="K58" s="107"/>
+      <c r="L58" s="107"/>
+      <c r="M58" s="108"/>
     </row>
     <row r="59" spans="2:13">
       <c r="B59" s="35" t="s">
@@ -2668,35 +2669,35 @@
       </c>
       <c r="E59" s="61">
         <f>+E16/D59</f>
-        <v>302.08463150000006</v>
+        <v>0</v>
       </c>
       <c r="F59" s="44">
         <v>6</v>
       </c>
       <c r="G59" s="61">
         <f>+G16/F59</f>
-        <v>197.75165699999999</v>
+        <v>0</v>
       </c>
       <c r="H59" s="44">
         <v>12</v>
       </c>
       <c r="I59" s="61">
         <f>+I16/H59</f>
-        <v>116.0707</v>
+        <v>0</v>
       </c>
       <c r="J59" s="44">
         <v>4</v>
       </c>
       <c r="K59" s="61">
         <f>+K16/J59</f>
-        <v>350.38158900000002</v>
+        <v>0</v>
       </c>
       <c r="L59" s="44">
         <v>6</v>
       </c>
       <c r="M59" s="61">
         <f>+M16/L59</f>
-        <v>243.28256666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:13">
@@ -2709,35 +2710,35 @@
       </c>
       <c r="E60" s="61">
         <f>+E16/D60</f>
-        <v>100.69487716666669</v>
+        <v>0</v>
       </c>
       <c r="F60" s="46">
         <v>12</v>
       </c>
       <c r="G60" s="61">
         <f>+G16/F60</f>
-        <v>98.875828499999997</v>
+        <v>0</v>
       </c>
       <c r="H60" s="45">
         <v>12</v>
       </c>
       <c r="I60" s="61">
         <f>+I16/H60</f>
-        <v>116.0707</v>
+        <v>0</v>
       </c>
       <c r="J60" s="45">
         <v>12</v>
       </c>
       <c r="K60" s="62">
         <f>+K16/J60</f>
-        <v>116.793863</v>
+        <v>0</v>
       </c>
       <c r="L60" s="45">
         <v>12</v>
       </c>
       <c r="M60" s="62">
         <f>+M16/L60</f>
-        <v>121.64128333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:13">
@@ -2758,53 +2759,130 @@
       <c r="D66" s="24"/>
     </row>
     <row r="67" spans="2:13">
-      <c r="B67" s="97" t="s">
+      <c r="B67" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="C67" s="98"/>
-      <c r="D67" s="98"/>
-      <c r="E67" s="98"/>
-      <c r="F67" s="98"/>
-      <c r="G67" s="98"/>
-      <c r="H67" s="99"/>
+      <c r="C67" s="77"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="77"/>
+      <c r="F67" s="77"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="78"/>
       <c r="M67" s="25"/>
     </row>
     <row r="68" spans="2:13">
-      <c r="B68" s="97" t="s">
+      <c r="B68" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="C68" s="98"/>
-      <c r="D68" s="98"/>
-      <c r="E68" s="98"/>
-      <c r="F68" s="98"/>
-      <c r="G68" s="98"/>
-      <c r="H68" s="99"/>
+      <c r="C68" s="77"/>
+      <c r="D68" s="77"/>
+      <c r="E68" s="77"/>
+      <c r="F68" s="77"/>
+      <c r="G68" s="77"/>
+      <c r="H68" s="78"/>
       <c r="M68" s="25"/>
     </row>
     <row r="69" spans="2:13">
-      <c r="B69" s="97" t="s">
+      <c r="B69" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C69" s="98"/>
-      <c r="D69" s="98"/>
-      <c r="E69" s="98"/>
-      <c r="F69" s="98"/>
-      <c r="G69" s="98"/>
-      <c r="H69" s="99"/>
+      <c r="C69" s="77"/>
+      <c r="D69" s="77"/>
+      <c r="E69" s="77"/>
+      <c r="F69" s="77"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="78"/>
     </row>
     <row r="70" spans="2:13">
-      <c r="B70" s="97" t="s">
+      <c r="B70" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C70" s="98"/>
-      <c r="D70" s="98"/>
-      <c r="E70" s="98"/>
-      <c r="F70" s="98"/>
-      <c r="G70" s="98"/>
-      <c r="H70" s="99"/>
+      <c r="C70" s="77"/>
+      <c r="D70" s="77"/>
+      <c r="E70" s="77"/>
+      <c r="F70" s="77"/>
+      <c r="G70" s="77"/>
+      <c r="H70" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="B58:M58"/>
+    <mergeCell ref="J38:K39"/>
+    <mergeCell ref="L38:M39"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J36:K37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F38:G39"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="H36:I37"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
@@ -2829,83 +2907,6 @@
     <mergeCell ref="L40:M40"/>
     <mergeCell ref="H38:I39"/>
     <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F38:G39"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="H36:I37"/>
-    <mergeCell ref="J36:K37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="B58:M58"/>
-    <mergeCell ref="J38:K39"/>
-    <mergeCell ref="L38:M39"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add buttons for export data & return (#31)
* feat: add buttons for export data & return

* feat: add design to detail view

---------

Co-authored-by: Bryan Martin Chilque <57159869+Ranzes33@users.noreply.github.com>
Co-authored-by: Paulo Llanos <37987149+paulo1403@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/rrggweb/resources/report_quotations.xlsx
+++ b/rrggweb/resources/report_quotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Riesgos\riesgosgenerales\rrggweb\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04671E7F-7C29-48AE-B941-2277CDF5DF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91445DA7-BDEF-4D52-8DF0-2EDDF72AD40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="135" windowWidth="19395" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18810" yWindow="135" windowWidth="19395" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -661,6 +661,69 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,21 +751,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -724,59 +775,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1560,16 +1560,16 @@
     <row r="12" spans="2:18" ht="75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="29"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="71"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="93"/>
+      <c r="M12" s="92"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="6" t="s">
@@ -1692,20 +1692,20 @@
       </c>
     </row>
     <row r="17" spans="2:13" ht="33" customHeight="1">
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="75"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="96"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="27"/>
@@ -1726,26 +1726,26 @@
         <v>5</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="79" t="s">
+      <c r="D19" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="80"/>
-      <c r="F19" s="79" t="s">
+      <c r="E19" s="84"/>
+      <c r="F19" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="80"/>
-      <c r="H19" s="79" t="s">
+      <c r="G19" s="84"/>
+      <c r="H19" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="80"/>
-      <c r="J19" s="79" t="s">
+      <c r="I19" s="84"/>
+      <c r="J19" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="80"/>
-      <c r="L19" s="79" t="s">
+      <c r="K19" s="84"/>
+      <c r="L19" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="M19" s="80"/>
+      <c r="M19" s="84"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="14" t="s">
@@ -1798,26 +1798,26 @@
         <v>9</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="100">
+      <c r="D23" s="70">
         <v>100000</v>
       </c>
-      <c r="E23" s="101"/>
-      <c r="F23" s="100">
+      <c r="E23" s="71"/>
+      <c r="F23" s="70">
         <v>180000</v>
       </c>
-      <c r="G23" s="101"/>
-      <c r="H23" s="100">
+      <c r="G23" s="71"/>
+      <c r="H23" s="70">
         <v>150000</v>
       </c>
-      <c r="I23" s="101"/>
-      <c r="J23" s="100">
+      <c r="I23" s="71"/>
+      <c r="J23" s="70">
         <v>150000</v>
       </c>
-      <c r="K23" s="101"/>
-      <c r="L23" s="100">
+      <c r="K23" s="71"/>
+      <c r="L23" s="70">
         <v>100000</v>
       </c>
-      <c r="M23" s="101"/>
+      <c r="M23" s="71"/>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="9" t="s">
@@ -1828,18 +1828,18 @@
       <c r="E24" s="12"/>
       <c r="F24" s="9"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="92" t="s">
+      <c r="H24" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="91"/>
-      <c r="J24" s="92" t="s">
+      <c r="I24" s="82"/>
+      <c r="J24" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="91"/>
-      <c r="L24" s="92" t="s">
+      <c r="K24" s="82"/>
+      <c r="L24" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="91"/>
+      <c r="M24" s="82"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="14"/>
@@ -1860,52 +1860,52 @@
         <v>9</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="100">
+      <c r="D26" s="70">
         <v>20000</v>
       </c>
-      <c r="E26" s="101"/>
-      <c r="F26" s="100">
+      <c r="E26" s="71"/>
+      <c r="F26" s="70">
         <v>30000</v>
       </c>
-      <c r="G26" s="101"/>
-      <c r="H26" s="100">
+      <c r="G26" s="71"/>
+      <c r="H26" s="70">
         <v>80000</v>
       </c>
-      <c r="I26" s="101"/>
-      <c r="J26" s="100">
+      <c r="I26" s="71"/>
+      <c r="J26" s="70">
         <v>50000</v>
       </c>
-      <c r="K26" s="101"/>
-      <c r="L26" s="100">
+      <c r="K26" s="71"/>
+      <c r="L26" s="70">
         <v>10000</v>
       </c>
-      <c r="M26" s="101"/>
+      <c r="M26" s="71"/>
     </row>
     <row r="27" spans="2:13">
       <c r="B27" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="92" t="s">
+      <c r="D27" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="91"/>
-      <c r="F27" s="92" t="s">
+      <c r="E27" s="82"/>
+      <c r="F27" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="91"/>
-      <c r="H27" s="92" t="s">
+      <c r="G27" s="82"/>
+      <c r="H27" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="91"/>
-      <c r="J27" s="92" t="s">
+      <c r="I27" s="82"/>
+      <c r="J27" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="91"/>
-      <c r="L27" s="92" t="s">
+      <c r="K27" s="82"/>
+      <c r="L27" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="M27" s="91"/>
+      <c r="M27" s="82"/>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="14"/>
@@ -1942,78 +1942,78 @@
         <v>16</v>
       </c>
       <c r="C30" s="15"/>
-      <c r="D30" s="100">
+      <c r="D30" s="70">
         <v>20000</v>
       </c>
-      <c r="E30" s="101"/>
-      <c r="F30" s="100">
+      <c r="E30" s="71"/>
+      <c r="F30" s="70">
         <v>20000</v>
       </c>
-      <c r="G30" s="101"/>
-      <c r="H30" s="100">
+      <c r="G30" s="71"/>
+      <c r="H30" s="70">
         <v>25000</v>
       </c>
-      <c r="I30" s="101"/>
-      <c r="J30" s="100">
+      <c r="I30" s="71"/>
+      <c r="J30" s="70">
         <v>25000</v>
       </c>
-      <c r="K30" s="101"/>
-      <c r="L30" s="100">
+      <c r="K30" s="71"/>
+      <c r="L30" s="70">
         <v>5000</v>
       </c>
-      <c r="M30" s="101"/>
+      <c r="M30" s="71"/>
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="15"/>
-      <c r="D31" s="100">
+      <c r="D31" s="70">
         <v>4000</v>
       </c>
-      <c r="E31" s="101"/>
-      <c r="F31" s="100">
+      <c r="E31" s="71"/>
+      <c r="F31" s="70">
         <v>4000</v>
       </c>
-      <c r="G31" s="101"/>
-      <c r="H31" s="100">
+      <c r="G31" s="71"/>
+      <c r="H31" s="70">
         <v>4000</v>
       </c>
-      <c r="I31" s="101"/>
-      <c r="J31" s="100">
+      <c r="I31" s="71"/>
+      <c r="J31" s="70">
         <v>4000</v>
       </c>
-      <c r="K31" s="101"/>
-      <c r="L31" s="100">
+      <c r="K31" s="71"/>
+      <c r="L31" s="70">
         <v>1000</v>
       </c>
-      <c r="M31" s="101"/>
+      <c r="M31" s="71"/>
     </row>
     <row r="32" spans="2:13">
       <c r="B32" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="15"/>
-      <c r="D32" s="100">
+      <c r="D32" s="70">
         <v>1000</v>
       </c>
-      <c r="E32" s="101"/>
-      <c r="F32" s="100">
+      <c r="E32" s="71"/>
+      <c r="F32" s="70">
         <v>1000</v>
       </c>
-      <c r="G32" s="101"/>
-      <c r="H32" s="100" t="s">
+      <c r="G32" s="71"/>
+      <c r="H32" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="I32" s="101"/>
-      <c r="J32" s="100">
+      <c r="I32" s="71"/>
+      <c r="J32" s="70">
         <v>2000</v>
       </c>
-      <c r="K32" s="101"/>
-      <c r="L32" s="100">
+      <c r="K32" s="71"/>
+      <c r="L32" s="70">
         <v>1000</v>
       </c>
-      <c r="M32" s="101"/>
+      <c r="M32" s="71"/>
     </row>
     <row r="33" spans="2:13" ht="8.25" customHeight="1">
       <c r="B33" s="51"/>
@@ -2034,26 +2034,26 @@
         <v>19</v>
       </c>
       <c r="C34" s="58"/>
-      <c r="D34" s="81" t="s">
+      <c r="D34" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="82"/>
-      <c r="F34" s="81" t="s">
+      <c r="E34" s="85"/>
+      <c r="F34" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="83"/>
-      <c r="H34" s="81" t="s">
+      <c r="G34" s="86"/>
+      <c r="H34" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="I34" s="83"/>
-      <c r="J34" s="81" t="s">
+      <c r="I34" s="86"/>
+      <c r="J34" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="83"/>
-      <c r="L34" s="82" t="s">
+      <c r="K34" s="86"/>
+      <c r="L34" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="M34" s="83"/>
+      <c r="M34" s="86"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="9"/>
@@ -2074,110 +2074,110 @@
         <v>21</v>
       </c>
       <c r="C36" s="55"/>
-      <c r="D36" s="96" t="s">
+      <c r="D36" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="97"/>
-      <c r="F36" s="104" t="s">
+      <c r="E36" s="76"/>
+      <c r="F36" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="104"/>
-      <c r="H36" s="96" t="s">
+      <c r="G36" s="79"/>
+      <c r="H36" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="I36" s="97"/>
-      <c r="J36" s="96" t="s">
+      <c r="I36" s="76"/>
+      <c r="J36" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="K36" s="97"/>
-      <c r="L36" s="104" t="s">
+      <c r="K36" s="76"/>
+      <c r="L36" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="M36" s="97"/>
+      <c r="M36" s="76"/>
     </row>
     <row r="37" spans="2:13">
       <c r="B37" s="56" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="57"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="105"/>
-      <c r="H37" s="98"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="105"/>
-      <c r="M37" s="99"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="80"/>
+      <c r="M37" s="78"/>
     </row>
     <row r="38" spans="2:13">
       <c r="B38" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C38" s="59"/>
-      <c r="D38" s="96" t="s">
+      <c r="D38" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="96" t="s">
+      <c r="E38" s="76"/>
+      <c r="F38" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="97"/>
-      <c r="H38" s="96" t="s">
+      <c r="G38" s="76"/>
+      <c r="H38" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="97"/>
-      <c r="J38" s="96" t="s">
+      <c r="I38" s="76"/>
+      <c r="J38" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="K38" s="97"/>
-      <c r="L38" s="104" t="s">
+      <c r="K38" s="76"/>
+      <c r="L38" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="M38" s="104"/>
+      <c r="M38" s="79"/>
     </row>
     <row r="39" spans="2:13">
       <c r="B39" s="56" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="60"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="98"/>
-      <c r="G39" s="99"/>
-      <c r="H39" s="98"/>
-      <c r="I39" s="99"/>
-      <c r="J39" s="98"/>
-      <c r="K39" s="99"/>
-      <c r="L39" s="105"/>
-      <c r="M39" s="105"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="78"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="78"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80"/>
     </row>
     <row r="40" spans="2:13">
       <c r="B40" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="93">
+      <c r="D40" s="87">
         <v>50000</v>
       </c>
-      <c r="E40" s="94"/>
-      <c r="F40" s="93">
+      <c r="E40" s="88"/>
+      <c r="F40" s="87">
         <v>50000</v>
       </c>
-      <c r="G40" s="94"/>
-      <c r="H40" s="102">
+      <c r="G40" s="88"/>
+      <c r="H40" s="89">
         <v>50000</v>
       </c>
-      <c r="I40" s="103"/>
-      <c r="J40" s="93">
+      <c r="I40" s="90"/>
+      <c r="J40" s="87">
         <v>50000</v>
       </c>
-      <c r="K40" s="94"/>
-      <c r="L40" s="95" t="s">
+      <c r="K40" s="88"/>
+      <c r="L40" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="M40" s="94"/>
+      <c r="M40" s="88"/>
     </row>
     <row r="41" spans="2:13">
       <c r="B41" s="9"/>
@@ -2198,56 +2198,56 @@
         <v>27</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="100">
+      <c r="D42" s="70">
         <v>250</v>
       </c>
-      <c r="E42" s="101"/>
-      <c r="F42" s="100">
+      <c r="E42" s="71"/>
+      <c r="F42" s="70">
         <v>250</v>
       </c>
-      <c r="G42" s="101"/>
-      <c r="H42" s="100">
+      <c r="G42" s="71"/>
+      <c r="H42" s="70">
         <v>500</v>
       </c>
-      <c r="I42" s="101"/>
-      <c r="J42" s="100">
+      <c r="I42" s="71"/>
+      <c r="J42" s="70">
         <v>250</v>
       </c>
-      <c r="K42" s="101">
+      <c r="K42" s="71">
         <v>250</v>
       </c>
-      <c r="L42" s="100">
+      <c r="L42" s="70">
         <v>250</v>
       </c>
-      <c r="M42" s="101"/>
+      <c r="M42" s="71"/>
     </row>
     <row r="43" spans="2:13">
       <c r="B43" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="100">
+      <c r="D43" s="70">
         <v>250</v>
       </c>
-      <c r="E43" s="101"/>
-      <c r="F43" s="100">
+      <c r="E43" s="71"/>
+      <c r="F43" s="70">
         <v>250</v>
       </c>
-      <c r="G43" s="101"/>
-      <c r="H43" s="100">
+      <c r="G43" s="71"/>
+      <c r="H43" s="70">
         <v>250</v>
       </c>
-      <c r="I43" s="101"/>
-      <c r="J43" s="100">
+      <c r="I43" s="71"/>
+      <c r="J43" s="70">
         <v>250</v>
       </c>
-      <c r="K43" s="101">
+      <c r="K43" s="71">
         <v>250</v>
       </c>
-      <c r="L43" s="100">
+      <c r="L43" s="70">
         <v>250</v>
       </c>
-      <c r="M43" s="101"/>
+      <c r="M43" s="71"/>
     </row>
     <row r="44" spans="2:13">
       <c r="B44" s="9"/>
@@ -2268,26 +2268,26 @@
         <v>29</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="100">
+      <c r="D45" s="70">
         <v>1000</v>
       </c>
-      <c r="E45" s="101"/>
-      <c r="F45" s="100">
+      <c r="E45" s="71"/>
+      <c r="F45" s="70">
         <v>500</v>
       </c>
-      <c r="G45" s="101"/>
-      <c r="H45" s="100">
+      <c r="G45" s="71"/>
+      <c r="H45" s="70">
         <v>1000</v>
       </c>
-      <c r="I45" s="101"/>
-      <c r="J45" s="100">
+      <c r="I45" s="71"/>
+      <c r="J45" s="70">
         <v>1000</v>
       </c>
-      <c r="K45" s="101"/>
-      <c r="L45" s="100">
+      <c r="K45" s="71"/>
+      <c r="L45" s="70">
         <v>500</v>
       </c>
-      <c r="M45" s="101"/>
+      <c r="M45" s="71"/>
     </row>
     <row r="46" spans="2:13">
       <c r="B46" s="14"/>
@@ -2308,68 +2308,68 @@
         <v>30</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="92" t="s">
+      <c r="D47" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="91"/>
-      <c r="F47" s="92" t="s">
+      <c r="E47" s="82"/>
+      <c r="F47" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="91"/>
-      <c r="H47" s="92" t="s">
+      <c r="G47" s="82"/>
+      <c r="H47" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="I47" s="91"/>
-      <c r="J47" s="92" t="s">
+      <c r="I47" s="82"/>
+      <c r="J47" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="K47" s="91"/>
-      <c r="L47" s="92" t="s">
+      <c r="K47" s="82"/>
+      <c r="L47" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="M47" s="91"/>
+      <c r="M47" s="82"/>
     </row>
     <row r="48" spans="2:13" ht="44.25" customHeight="1">
       <c r="B48" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C48" s="33"/>
-      <c r="D48" s="92" t="s">
+      <c r="D48" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="91"/>
-      <c r="F48" s="92" t="s">
+      <c r="E48" s="82"/>
+      <c r="F48" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="91"/>
-      <c r="H48" s="92" t="s">
+      <c r="G48" s="82"/>
+      <c r="H48" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="I48" s="91"/>
-      <c r="J48" s="79" t="s">
+      <c r="I48" s="82"/>
+      <c r="J48" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="K48" s="80"/>
-      <c r="L48" s="92" t="s">
+      <c r="K48" s="84"/>
+      <c r="L48" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="M48" s="91"/>
+      <c r="M48" s="82"/>
     </row>
     <row r="49" spans="2:13" ht="19.5" customHeight="1">
-      <c r="B49" s="84" t="s">
+      <c r="B49" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="86"/>
-      <c r="I49" s="86"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="85"/>
-      <c r="M49" s="87"/>
+      <c r="C49" s="102"/>
+      <c r="D49" s="102"/>
+      <c r="E49" s="102"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="102"/>
+      <c r="H49" s="103"/>
+      <c r="I49" s="103"/>
+      <c r="J49" s="102"/>
+      <c r="K49" s="102"/>
+      <c r="L49" s="102"/>
+      <c r="M49" s="104"/>
     </row>
     <row r="50" spans="2:13">
       <c r="B50" s="27" t="s">
@@ -2588,36 +2588,36 @@
         <v>46</v>
       </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="92" t="s">
+      <c r="D56" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="E56" s="91"/>
-      <c r="F56" s="92" t="s">
+      <c r="E56" s="82"/>
+      <c r="F56" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G56" s="91"/>
-      <c r="H56" s="92" t="s">
+      <c r="G56" s="82"/>
+      <c r="H56" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="I56" s="91"/>
-      <c r="J56" s="90" t="s">
+      <c r="I56" s="82"/>
+      <c r="J56" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="K56" s="91"/>
-      <c r="L56" s="92" t="s">
+      <c r="K56" s="82"/>
+      <c r="L56" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="M56" s="91"/>
+      <c r="M56" s="82"/>
     </row>
     <row r="57" spans="2:13" ht="33" customHeight="1">
       <c r="B57" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C57" s="37"/>
-      <c r="D57" s="88" t="s">
+      <c r="D57" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="89"/>
+      <c r="E57" s="106"/>
       <c r="F57" s="20">
         <v>0.2</v>
       </c>
@@ -2644,20 +2644,20 @@
       </c>
     </row>
     <row r="58" spans="2:13" ht="25.5" customHeight="1">
-      <c r="B58" s="106" t="s">
+      <c r="B58" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="107"/>
-      <c r="D58" s="107"/>
-      <c r="E58" s="107"/>
-      <c r="F58" s="107"/>
-      <c r="G58" s="107"/>
-      <c r="H58" s="107"/>
-      <c r="I58" s="107"/>
-      <c r="J58" s="107"/>
-      <c r="K58" s="107"/>
-      <c r="L58" s="107"/>
-      <c r="M58" s="108"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="73"/>
+      <c r="K58" s="73"/>
+      <c r="L58" s="73"/>
+      <c r="M58" s="74"/>
     </row>
     <row r="59" spans="2:13">
       <c r="B59" s="35" t="s">
@@ -2759,53 +2759,130 @@
       <c r="D66" s="24"/>
     </row>
     <row r="67" spans="2:13">
-      <c r="B67" s="76" t="s">
+      <c r="B67" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="C67" s="77"/>
-      <c r="D67" s="77"/>
-      <c r="E67" s="77"/>
-      <c r="F67" s="77"/>
-      <c r="G67" s="77"/>
-      <c r="H67" s="78"/>
+      <c r="C67" s="98"/>
+      <c r="D67" s="98"/>
+      <c r="E67" s="98"/>
+      <c r="F67" s="98"/>
+      <c r="G67" s="98"/>
+      <c r="H67" s="99"/>
       <c r="M67" s="25"/>
     </row>
     <row r="68" spans="2:13">
-      <c r="B68" s="76" t="s">
+      <c r="B68" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="C68" s="77"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="77"/>
-      <c r="F68" s="77"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="78"/>
+      <c r="C68" s="98"/>
+      <c r="D68" s="98"/>
+      <c r="E68" s="98"/>
+      <c r="F68" s="98"/>
+      <c r="G68" s="98"/>
+      <c r="H68" s="99"/>
       <c r="M68" s="25"/>
     </row>
     <row r="69" spans="2:13">
-      <c r="B69" s="76" t="s">
+      <c r="B69" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="C69" s="77"/>
-      <c r="D69" s="77"/>
-      <c r="E69" s="77"/>
-      <c r="F69" s="77"/>
-      <c r="G69" s="77"/>
-      <c r="H69" s="78"/>
+      <c r="C69" s="98"/>
+      <c r="D69" s="98"/>
+      <c r="E69" s="98"/>
+      <c r="F69" s="98"/>
+      <c r="G69" s="98"/>
+      <c r="H69" s="99"/>
     </row>
     <row r="70" spans="2:13">
-      <c r="B70" s="76" t="s">
+      <c r="B70" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="C70" s="77"/>
-      <c r="D70" s="77"/>
-      <c r="E70" s="77"/>
-      <c r="F70" s="77"/>
-      <c r="G70" s="77"/>
-      <c r="H70" s="78"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="98"/>
+      <c r="E70" s="98"/>
+      <c r="F70" s="98"/>
+      <c r="G70" s="98"/>
+      <c r="H70" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B49:M49"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L56:M56"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="H38:I39"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F38:G39"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="H36:I37"/>
+    <mergeCell ref="J36:K37"/>
+    <mergeCell ref="L36:M37"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
     <mergeCell ref="J45:K45"/>
     <mergeCell ref="L45:M45"/>
     <mergeCell ref="B58:M58"/>
@@ -2830,83 +2907,6 @@
     <mergeCell ref="H47:I47"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J36:K37"/>
-    <mergeCell ref="L36:M37"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F38:G39"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="H36:I37"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B49:M49"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="L56:M56"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="H38:I39"/>
-    <mergeCell ref="J34:K34"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>